<commit_message>
Replaced sound with Miata sound
</commit_message>
<xml_diff>
--- a/AC Worksheet v016.xlsx
+++ b/AC Worksheet v016.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Documents\LostInTranslationViewtModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EBB069B-DBB6-491F-B5F9-9BB1E97E7997}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8780DAC-1155-4709-A2C6-2161F12F27E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="30912" windowHeight="16752" tabRatio="629" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38265" yWindow="5715" windowWidth="25470" windowHeight="16020" tabRatio="629" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="2" r:id="rId1"/>
@@ -1269,52 +1269,52 @@
     <t>Input the torque values, either in kp, ft-lb or NM and adjust the drivetrain loss if needed. The formula will generate a power.lut</t>
   </si>
   <si>
-    <t>0|7</t>
-  </si>
-  <si>
-    <t>500|7</t>
-  </si>
-  <si>
-    <t>1000|14</t>
-  </si>
-  <si>
-    <t>1500|22</t>
-  </si>
-  <si>
-    <t>2000|29</t>
-  </si>
-  <si>
-    <t>2500|37</t>
-  </si>
-  <si>
-    <t>3000|40</t>
-  </si>
-  <si>
-    <t>3500|43</t>
-  </si>
-  <si>
-    <t>4000|43</t>
-  </si>
-  <si>
-    <t>4500|42</t>
-  </si>
-  <si>
-    <t>5000|38</t>
-  </si>
-  <si>
-    <t>5500|37</t>
-  </si>
-  <si>
-    <t>6000|34</t>
-  </si>
-  <si>
-    <t>6500|31</t>
-  </si>
-  <si>
     <t>TRMotorsport  C1</t>
   </si>
   <si>
     <t>Hankook  Ventus R-S4</t>
+  </si>
+  <si>
+    <t>0|9</t>
+  </si>
+  <si>
+    <t>500|9</t>
+  </si>
+  <si>
+    <t>1000|19</t>
+  </si>
+  <si>
+    <t>1500|29</t>
+  </si>
+  <si>
+    <t>2000|39</t>
+  </si>
+  <si>
+    <t>2500|50</t>
+  </si>
+  <si>
+    <t>3000|54</t>
+  </si>
+  <si>
+    <t>3500|57</t>
+  </si>
+  <si>
+    <t>4000|57</t>
+  </si>
+  <si>
+    <t>4500|56</t>
+  </si>
+  <si>
+    <t>5000|51</t>
+  </si>
+  <si>
+    <t>5500|50</t>
+  </si>
+  <si>
+    <t>6000|46</t>
+  </si>
+  <si>
+    <t>6500|42</t>
   </si>
 </sst>
 </file>
@@ -3751,46 +3751,46 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="37"/>
                 <c:pt idx="0">
-                  <c:v>7.35498750274897</c:v>
+                  <c:v>9.8066500036652933</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.35498750274897</c:v>
+                  <c:v>9.8066500036652933</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14.70997500549794</c:v>
+                  <c:v>19.613300007330587</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>22.064962508246911</c:v>
+                  <c:v>29.41995001099588</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>29.41995001099588</c:v>
+                  <c:v>39.226600014661173</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>37.623948080310001</c:v>
+                  <c:v>50.165264107079999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>40.674538465200001</c:v>
+                  <c:v>54.232717953600002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43.216697119274997</c:v>
+                  <c:v>57.622262825699998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43.216697119274997</c:v>
+                  <c:v>57.622262825699998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>42.199833657645001</c:v>
+                  <c:v>56.26644487686</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>38.640811541939996</c:v>
+                  <c:v>51.521082055919997</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>37.623948080310001</c:v>
+                  <c:v>50.165264107079999</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>34.57335769542</c:v>
+                  <c:v>46.097810260559996</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>31.52276731053</c:v>
+                  <c:v>42.03035641404</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0</c:v>
@@ -7479,9 +7479,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1114425</xdr:colOff>
+      <xdr:colOff>1120140</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>87351</xdr:rowOff>
+      <xdr:rowOff>93066</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7529,9 +7529,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>447674</xdr:colOff>
+      <xdr:colOff>441959</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>164454</xdr:rowOff>
+      <xdr:rowOff>172074</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -12432,8 +12432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AJ55"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L31" sqref="L18:L31"/>
+    <sheetView topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18:L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13223,18 +13223,18 @@
         <v>0.68965773391293606</v>
       </c>
       <c r="I18" s="77">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="J18" s="72">
         <f>J19</f>
-        <v>7.35498750274897</v>
+        <v>9.8066500036652933</v>
       </c>
       <c r="K18" s="22" t="str">
         <f t="shared" ref="K18:K54" si="0">CONCATENATE(D18,"|",INT(J18))</f>
-        <v>0|7</v>
+        <v>0|9</v>
       </c>
       <c r="L18" s="6" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="M18" s="16"/>
       <c r="N18" s="16"/>
@@ -13284,18 +13284,18 @@
         <v>0.68965773391293606</v>
       </c>
       <c r="I19" s="78">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="J19" s="72">
         <f>G19*(1-I19)</f>
-        <v>7.35498750274897</v>
+        <v>9.8066500036652933</v>
       </c>
       <c r="K19" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>500|7</v>
+        <v>500|9</v>
       </c>
       <c r="L19" s="6" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="M19" s="16"/>
       <c r="N19" s="16"/>
@@ -13346,18 +13346,18 @@
         <v>2.7586309356517442</v>
       </c>
       <c r="I20" s="79">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="J20" s="72">
         <f t="shared" ref="J20:J54" si="4">G20*(1-I20)</f>
-        <v>14.70997500549794</v>
+        <v>19.613300007330587</v>
       </c>
       <c r="K20" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>1000|14</v>
+        <v>1000|19</v>
       </c>
       <c r="L20" s="6" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="M20" s="16"/>
       <c r="N20" s="16"/>
@@ -13408,18 +13408,18 @@
         <v>6.2069196052164237</v>
       </c>
       <c r="I21" s="79">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="J21" s="72">
         <f t="shared" si="4"/>
-        <v>22.064962508246911</v>
+        <v>29.41995001099588</v>
       </c>
       <c r="K21" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>1500|22</v>
+        <v>1500|29</v>
       </c>
       <c r="L21" s="6" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="M21" s="16"/>
       <c r="N21" s="16"/>
@@ -13470,18 +13470,18 @@
         <v>11.034523742606977</v>
       </c>
       <c r="I22" s="79">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="J22" s="72">
         <f t="shared" si="4"/>
-        <v>29.41995001099588</v>
+        <v>39.226600014661173</v>
       </c>
       <c r="K22" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>2000|29</v>
+        <v>2000|39</v>
       </c>
       <c r="L22" s="6" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="M22" s="16"/>
       <c r="N22" s="16"/>
@@ -13533,18 +13533,18 @@
         <v>17.639490729404002</v>
       </c>
       <c r="I23" s="79">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="J23" s="72">
         <f t="shared" si="4"/>
-        <v>37.623948080310001</v>
+        <v>50.165264107079999</v>
       </c>
       <c r="K23" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>2500|37</v>
+        <v>2500|50</v>
       </c>
       <c r="L23" s="6" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="M23" s="16"/>
       <c r="N23" s="16"/>
@@ -13596,18 +13596,18 @@
         <v>22.883663648956546</v>
       </c>
       <c r="I24" s="79">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="J24" s="72">
         <f t="shared" si="4"/>
-        <v>40.674538465200001</v>
+        <v>54.232717953600002</v>
       </c>
       <c r="K24" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>3000|40</v>
+        <v>3000|54</v>
       </c>
       <c r="L24" s="6" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="M24" s="16"/>
       <c r="N24" s="16"/>
@@ -13659,18 +13659,18 @@
         <v>28.366208064852383</v>
       </c>
       <c r="I25" s="79">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="J25" s="72">
         <f t="shared" si="4"/>
-        <v>43.216697119274997</v>
+        <v>57.622262825699998</v>
       </c>
       <c r="K25" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>3500|43</v>
+        <v>3500|57</v>
       </c>
       <c r="L25" s="6" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="M25" s="16"/>
       <c r="N25" s="16"/>
@@ -13722,18 +13722,18 @@
         <v>32.418523502688444</v>
       </c>
       <c r="I26" s="79">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="J26" s="72">
         <f t="shared" si="4"/>
-        <v>43.216697119274997</v>
+        <v>57.622262825699998</v>
       </c>
       <c r="K26" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>4000|43</v>
+        <v>4000|57</v>
       </c>
       <c r="L26" s="6" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="M26" s="16"/>
       <c r="N26" s="16"/>
@@ -13785,18 +13785,18 @@
         <v>35.612701553688623</v>
       </c>
       <c r="I27" s="79">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="J27" s="72">
         <f t="shared" si="4"/>
-        <v>42.199833657645001</v>
+        <v>56.26644487686</v>
       </c>
       <c r="K27" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>4500|42</v>
+        <v>4500|56</v>
       </c>
       <c r="L27" s="6" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="M27" s="16"/>
       <c r="N27" s="16"/>
@@ -13848,18 +13848,18 @@
         <v>36.232467444181196</v>
       </c>
       <c r="I28" s="79">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="J28" s="72">
         <f t="shared" si="4"/>
-        <v>38.640811541939996</v>
+        <v>51.521082055919997</v>
       </c>
       <c r="K28" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>5000|38</v>
+        <v>5000|51</v>
       </c>
       <c r="L28" s="6" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="M28" s="16"/>
       <c r="N28" s="16"/>
@@ -13911,18 +13911,18 @@
         <v>38.806879604688802</v>
       </c>
       <c r="I29" s="79">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="J29" s="72">
         <f t="shared" si="4"/>
-        <v>37.623948080310001</v>
+        <v>50.165264107079999</v>
       </c>
       <c r="K29" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>5500|37</v>
+        <v>5500|50</v>
       </c>
       <c r="L29" s="6" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="M29" s="16"/>
       <c r="N29" s="16"/>
@@ -13974,18 +13974,18 @@
         <v>38.90222820322613</v>
       </c>
       <c r="I30" s="79">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="J30" s="72">
         <f t="shared" si="4"/>
-        <v>34.57335769542</v>
+        <v>46.097810260559996</v>
       </c>
       <c r="K30" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>6000|34</v>
+        <v>6000|46</v>
       </c>
       <c r="L30" s="6" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="M30" s="16"/>
       <c r="N30" s="16"/>
@@ -14037,18 +14037,18 @@
         <v>38.425485210539534</v>
       </c>
       <c r="I31" s="79">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="J31" s="72">
         <f t="shared" si="4"/>
-        <v>31.52276731053</v>
+        <v>42.03035641404</v>
       </c>
       <c r="K31" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>6500|31</v>
+        <v>6500|42</v>
       </c>
       <c r="L31" s="6" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="M31" s="16"/>
       <c r="N31" s="16"/>
@@ -14100,7 +14100,7 @@
       </c>
       <c r="I32" s="79">
         <f t="shared" ref="I32:I54" si="6">I31</f>
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="J32" s="72">
         <f t="shared" si="4"/>
@@ -14161,7 +14161,7 @@
       </c>
       <c r="I33" s="79">
         <f t="shared" si="6"/>
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="J33" s="72">
         <f t="shared" si="4"/>
@@ -14222,7 +14222,7 @@
       </c>
       <c r="I34" s="79">
         <f t="shared" si="6"/>
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="J34" s="72">
         <f t="shared" si="4"/>
@@ -14283,7 +14283,7 @@
       </c>
       <c r="I35" s="79">
         <f t="shared" si="6"/>
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="J35" s="72">
         <f t="shared" si="4"/>
@@ -14344,7 +14344,7 @@
       </c>
       <c r="I36" s="79">
         <f t="shared" si="6"/>
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="J36" s="72">
         <f t="shared" si="4"/>
@@ -14405,7 +14405,7 @@
       </c>
       <c r="I37" s="79">
         <f t="shared" si="6"/>
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="J37" s="72">
         <f t="shared" si="4"/>
@@ -14466,7 +14466,7 @@
       </c>
       <c r="I38" s="79">
         <f t="shared" si="6"/>
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="J38" s="72">
         <f t="shared" si="4"/>
@@ -14527,7 +14527,7 @@
       </c>
       <c r="I39" s="79">
         <f t="shared" si="6"/>
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="J39" s="72">
         <f t="shared" si="4"/>
@@ -14588,7 +14588,7 @@
       </c>
       <c r="I40" s="79">
         <f t="shared" si="6"/>
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="J40" s="72">
         <f t="shared" si="4"/>
@@ -14649,7 +14649,7 @@
       </c>
       <c r="I41" s="79">
         <f t="shared" si="6"/>
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="J41" s="72">
         <f t="shared" si="4"/>
@@ -14710,7 +14710,7 @@
       </c>
       <c r="I42" s="79">
         <f t="shared" si="6"/>
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="J42" s="72">
         <f t="shared" si="4"/>
@@ -14771,7 +14771,7 @@
       </c>
       <c r="I43" s="79">
         <f t="shared" si="6"/>
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="J43" s="72">
         <f t="shared" si="4"/>
@@ -14832,7 +14832,7 @@
       </c>
       <c r="I44" s="79">
         <f t="shared" si="6"/>
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="J44" s="72">
         <f t="shared" si="4"/>
@@ -14893,7 +14893,7 @@
       </c>
       <c r="I45" s="79">
         <f t="shared" si="6"/>
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="J45" s="72">
         <f t="shared" si="4"/>
@@ -14954,7 +14954,7 @@
       </c>
       <c r="I46" s="79">
         <f t="shared" si="6"/>
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="J46" s="72">
         <f t="shared" si="4"/>
@@ -15015,7 +15015,7 @@
       </c>
       <c r="I47" s="79">
         <f t="shared" si="6"/>
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="J47" s="72">
         <f t="shared" si="4"/>
@@ -15076,7 +15076,7 @@
       </c>
       <c r="I48" s="79">
         <f t="shared" si="6"/>
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="J48" s="72">
         <f t="shared" si="4"/>
@@ -15137,7 +15137,7 @@
       </c>
       <c r="I49" s="79">
         <f t="shared" si="6"/>
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="J49" s="72">
         <f t="shared" si="4"/>
@@ -15198,7 +15198,7 @@
       </c>
       <c r="I50" s="79">
         <f t="shared" si="6"/>
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="J50" s="72">
         <f t="shared" si="4"/>
@@ -15259,7 +15259,7 @@
       </c>
       <c r="I51" s="79">
         <f t="shared" si="6"/>
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="J51" s="72">
         <f t="shared" si="4"/>
@@ -15320,7 +15320,7 @@
       </c>
       <c r="I52" s="79">
         <f t="shared" si="6"/>
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="J52" s="72">
         <f t="shared" si="4"/>
@@ -15381,7 +15381,7 @@
       </c>
       <c r="I53" s="79">
         <f t="shared" si="6"/>
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="J53" s="72">
         <f t="shared" si="4"/>
@@ -15442,7 +15442,7 @@
       </c>
       <c r="I54" s="79">
         <f t="shared" si="6"/>
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="J54" s="72">
         <f t="shared" si="4"/>
@@ -29329,7 +29329,7 @@
   <dimension ref="A1:X60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -29430,7 +29430,7 @@
         <v>285</v>
       </c>
       <c r="D3" s="298" t="s">
-        <v>409</v>
+        <v>395</v>
       </c>
       <c r="E3" s="297">
         <v>15</v>
@@ -29473,7 +29473,7 @@
         <v>286</v>
       </c>
       <c r="D4" s="298" t="s">
-        <v>409</v>
+        <v>395</v>
       </c>
       <c r="E4" s="297">
         <v>15</v>
@@ -29588,7 +29588,7 @@
         <v>285</v>
       </c>
       <c r="D7" s="298" t="s">
-        <v>410</v>
+        <v>396</v>
       </c>
       <c r="E7" s="297">
         <v>195</v>
@@ -29603,11 +29603,11 @@
         <v>576</v>
       </c>
       <c r="I7" s="312">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="J7" s="312">
         <f>I7*0.45359237</f>
-        <v>11.33980925</v>
+        <v>8.6182550300000003</v>
       </c>
       <c r="K7" s="311">
         <v>51</v>
@@ -29633,7 +29633,7 @@
         <v>286</v>
       </c>
       <c r="D8" s="298" t="s">
-        <v>410</v>
+        <v>396</v>
       </c>
       <c r="E8" s="297">
         <v>195</v>
@@ -29648,11 +29648,11 @@
         <v>576</v>
       </c>
       <c r="I8" s="312">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="J8" s="312">
         <f>I8*0.45359237</f>
-        <v>11.33980925</v>
+        <v>8.6182550300000003</v>
       </c>
       <c r="K8" s="311">
         <v>51</v>
@@ -29742,11 +29742,11 @@
       </c>
       <c r="E11" s="303">
         <f>0.5*M20*M16^2</f>
-        <v>0.52404281540661801</v>
+        <v>0.44086141613572621</v>
       </c>
       <c r="F11" s="303">
         <f>0.5*N20*N16^2</f>
-        <v>0.52404281540661801</v>
+        <v>0.44086141613572621</v>
       </c>
       <c r="G11" s="306"/>
       <c r="H11" s="177"/>
@@ -29776,11 +29776,11 @@
       </c>
       <c r="E12" s="303">
         <f>(0.5*M18*M14^2)+(0.5*M19*(M14^2+M16^2))</f>
-        <v>0.5758690549330634</v>
+        <v>0.45629402212179893</v>
       </c>
       <c r="F12" s="303">
         <f>(0.5*N18*N14^2)+(0.5*N19*(N14^2+N16^2))</f>
-        <v>0.5758690549330634</v>
+        <v>0.45629402212179893</v>
       </c>
       <c r="G12" s="307"/>
       <c r="H12" s="177"/>
@@ -29810,11 +29810,11 @@
       </c>
       <c r="E13" s="304">
         <f>(0.66666*M18*M14^2)+(0.66666*M19*(M14^2+M16^2))</f>
-        <v>0.76781772832335227</v>
+        <v>0.60838594557543701</v>
       </c>
       <c r="F13" s="304">
         <f>(0.66666*N18*N14^2)+(0.66666*N19*(N14^2+N16^2))</f>
-        <v>0.76781772832335227</v>
+        <v>0.60838594557543701</v>
       </c>
       <c r="G13" s="145"/>
       <c r="H13" s="16"/>
@@ -30026,11 +30026,11 @@
       </c>
       <c r="M19" s="309">
         <f>I7/32.2</f>
-        <v>0.77639751552795022</v>
+        <v>0.59006211180124213</v>
       </c>
       <c r="N19" s="309">
         <f>I8/32.2</f>
-        <v>0.77639751552795022</v>
+        <v>0.59006211180124213</v>
       </c>
       <c r="O19" s="16"/>
       <c r="P19" s="16"/>
@@ -30060,11 +30060,11 @@
       </c>
       <c r="M20" s="309">
         <f>M19+M18</f>
-        <v>1.1739130434782608</v>
+        <v>0.98757763975155266</v>
       </c>
       <c r="N20" s="309">
         <f>N19+N18</f>
-        <v>1.1739130434782608</v>
+        <v>0.98757763975155266</v>
       </c>
       <c r="O20" s="16"/>
       <c r="P20" s="16"/>

</xml_diff>

<commit_message>
ChatGPT-interpolated torque curve below what I have on the dyno chart (amusingly it ended up with the same values I'd guessed)
</commit_message>
<xml_diff>
--- a/AC Worksheet v016.xlsx
+++ b/AC Worksheet v016.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\Documents\LostInTranslationViewtModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8780DAC-1155-4709-A2C6-2161F12F27E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67F43807-247E-4BE8-A5C6-C346497D5979}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38265" yWindow="5715" windowWidth="25470" windowHeight="16020" tabRatio="629" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" tabRatio="629" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="2" r:id="rId1"/>
@@ -1275,21 +1275,6 @@
     <t>Hankook  Ventus R-S4</t>
   </si>
   <si>
-    <t>0|9</t>
-  </si>
-  <si>
-    <t>500|9</t>
-  </si>
-  <si>
-    <t>1000|19</t>
-  </si>
-  <si>
-    <t>1500|29</t>
-  </si>
-  <si>
-    <t>2000|39</t>
-  </si>
-  <si>
     <t>2500|50</t>
   </si>
   <si>
@@ -1315,6 +1300,21 @@
   </si>
   <si>
     <t>6500|42</t>
+  </si>
+  <si>
+    <t>0|12</t>
+  </si>
+  <si>
+    <t>500|12</t>
+  </si>
+  <si>
+    <t>1000|18</t>
+  </si>
+  <si>
+    <t>1500|28</t>
+  </si>
+  <si>
+    <t>2000|37</t>
   </si>
 </sst>
 </file>
@@ -3468,19 +3468,19 @@
                 <c:formatCode>_-* #,##0_-;\-* #,##0_-;_-* "-"??_-;_-@_-</c:formatCode>
                 <c:ptCount val="37"/>
                 <c:pt idx="0">
-                  <c:v>0.68965773391293606</c:v>
+                  <c:v>0.8581373868358706</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.68965773391293606</c:v>
+                  <c:v>0.8581373868358706</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.7586309356517442</c:v>
+                  <c:v>2.6697607590449302</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.2069196052164237</c:v>
+                  <c:v>6.0069617078510937</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11.034523742606977</c:v>
+                  <c:v>10.679043036179721</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>17.639490729404002</c:v>
@@ -3751,19 +3751,19 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="37"/>
                 <c:pt idx="0">
-                  <c:v>9.8066500036652933</c:v>
+                  <c:v>12.20236153956</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.8066500036652933</c:v>
+                  <c:v>12.20236153956</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>19.613300007330587</c:v>
+                  <c:v>18.981451283759998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>29.41995001099588</c:v>
+                  <c:v>28.472176925639999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>39.226600014661173</c:v>
+                  <c:v>37.962902567519997</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>50.165264107079999</c:v>
@@ -3892,19 +3892,19 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="37"/>
                 <c:pt idx="0">
-                  <c:v>9.8066500036652933</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.8066500036652933</c:v>
+                  <c:v>12.20236153956</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>19.613300007330587</c:v>
+                  <c:v>18.981451283759998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>29.41995001099588</c:v>
+                  <c:v>28.472176925639999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>39.226600014661173</c:v>
+                  <c:v>37.962902567519997</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>50.165264107079999</c:v>
@@ -12432,8 +12432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AJ55"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18:L31"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L34" sqref="L34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13208,33 +13208,32 @@
       </c>
       <c r="E18" s="74">
         <f>E19</f>
-        <v>1</v>
+        <v>1.244294589385702</v>
       </c>
       <c r="F18" s="74">
-        <f>F19</f>
-        <v>7.2330138512</v>
+        <v>0</v>
       </c>
       <c r="G18" s="75">
         <f>F18*1.35581794884</f>
-        <v>9.8066500036652933</v>
+        <v>0</v>
       </c>
       <c r="H18" s="69">
         <f>H19</f>
-        <v>0.68965773391293606</v>
+        <v>0.8581373868358706</v>
       </c>
       <c r="I18" s="77">
         <v>0</v>
       </c>
       <c r="J18" s="72">
         <f>J19</f>
-        <v>9.8066500036652933</v>
+        <v>12.20236153956</v>
       </c>
       <c r="K18" s="22" t="str">
         <f t="shared" ref="K18:K54" si="0">CONCATENATE(D18,"|",INT(J18))</f>
-        <v>0|9</v>
+        <v>0|12</v>
       </c>
       <c r="L18" s="6" t="s">
-        <v>397</v>
+        <v>406</v>
       </c>
       <c r="M18" s="16"/>
       <c r="N18" s="16"/>
@@ -13269,33 +13268,34 @@
         <v>500</v>
       </c>
       <c r="E19" s="61">
-        <v>1</v>
+        <f>9/7.2330138512</f>
+        <v>1.244294589385702</v>
       </c>
       <c r="F19" s="61">
         <f t="shared" ref="F19:F54" si="1">E19*7.2330138512</f>
-        <v>7.2330138512</v>
+        <v>9</v>
       </c>
       <c r="G19" s="62">
         <f>F19*1.35581794884</f>
-        <v>9.8066500036652933</v>
+        <v>12.20236153956</v>
       </c>
       <c r="H19" s="69">
         <f t="shared" ref="H19:H54" si="2">G19*0.101972*D19/725</f>
-        <v>0.68965773391293606</v>
+        <v>0.8581373868358706</v>
       </c>
       <c r="I19" s="78">
         <v>0</v>
       </c>
       <c r="J19" s="72">
         <f>G19*(1-I19)</f>
-        <v>9.8066500036652933</v>
+        <v>12.20236153956</v>
       </c>
       <c r="K19" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>500|9</v>
+        <v>500|12</v>
       </c>
       <c r="L19" s="6" t="s">
-        <v>398</v>
+        <v>407</v>
       </c>
       <c r="M19" s="16"/>
       <c r="N19" s="16"/>
@@ -13331,33 +13331,34 @@
         <v>1000</v>
       </c>
       <c r="E20" s="61">
-        <v>2</v>
+        <f>14/7.2330138512</f>
+        <v>1.9355693612666478</v>
       </c>
       <c r="F20" s="61">
         <f t="shared" si="1"/>
-        <v>14.4660277024</v>
+        <v>14</v>
       </c>
       <c r="G20" s="62">
         <f t="shared" ref="G20:G54" si="3">F20*1.35581794884</f>
-        <v>19.613300007330587</v>
+        <v>18.981451283759998</v>
       </c>
       <c r="H20" s="69">
         <f t="shared" si="2"/>
-        <v>2.7586309356517442</v>
+        <v>2.6697607590449302</v>
       </c>
       <c r="I20" s="79">
         <v>0</v>
       </c>
       <c r="J20" s="72">
         <f t="shared" ref="J20:J54" si="4">G20*(1-I20)</f>
-        <v>19.613300007330587</v>
+        <v>18.981451283759998</v>
       </c>
       <c r="K20" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>1000|19</v>
+        <v>1000|18</v>
       </c>
       <c r="L20" s="6" t="s">
-        <v>399</v>
+        <v>408</v>
       </c>
       <c r="M20" s="16"/>
       <c r="N20" s="16"/>
@@ -13393,33 +13394,34 @@
         <v>1500</v>
       </c>
       <c r="E21" s="61">
-        <v>3</v>
+        <f>21/7.2330138512</f>
+        <v>2.9033540418999717</v>
       </c>
       <c r="F21" s="61">
         <f t="shared" si="1"/>
-        <v>21.699041553600001</v>
+        <v>21</v>
       </c>
       <c r="G21" s="62">
         <f t="shared" si="3"/>
-        <v>29.41995001099588</v>
+        <v>28.472176925639999</v>
       </c>
       <c r="H21" s="69">
         <f t="shared" si="2"/>
-        <v>6.2069196052164237</v>
+        <v>6.0069617078510937</v>
       </c>
       <c r="I21" s="79">
         <v>0</v>
       </c>
       <c r="J21" s="72">
         <f t="shared" si="4"/>
-        <v>29.41995001099588</v>
+        <v>28.472176925639999</v>
       </c>
       <c r="K21" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>1500|29</v>
+        <v>1500|28</v>
       </c>
       <c r="L21" s="6" t="s">
-        <v>400</v>
+        <v>409</v>
       </c>
       <c r="M21" s="16"/>
       <c r="N21" s="16"/>
@@ -13455,33 +13457,34 @@
         <v>2000</v>
       </c>
       <c r="E22" s="61">
-        <v>4</v>
+        <f>28/7.2330138512</f>
+        <v>3.8711387225332956</v>
       </c>
       <c r="F22" s="61">
         <f t="shared" si="1"/>
-        <v>28.9320554048</v>
+        <v>28</v>
       </c>
       <c r="G22" s="62">
         <f t="shared" si="3"/>
-        <v>39.226600014661173</v>
+        <v>37.962902567519997</v>
       </c>
       <c r="H22" s="69">
         <f t="shared" si="2"/>
-        <v>11.034523742606977</v>
+        <v>10.679043036179721</v>
       </c>
       <c r="I22" s="79">
         <v>0</v>
       </c>
       <c r="J22" s="72">
         <f t="shared" si="4"/>
-        <v>39.226600014661173</v>
+        <v>37.962902567519997</v>
       </c>
       <c r="K22" s="22" t="str">
         <f t="shared" si="0"/>
-        <v>2000|39</v>
+        <v>2000|37</v>
       </c>
       <c r="L22" s="6" t="s">
-        <v>401</v>
+        <v>410</v>
       </c>
       <c r="M22" s="16"/>
       <c r="N22" s="16"/>
@@ -13544,7 +13547,7 @@
         <v>2500|50</v>
       </c>
       <c r="L23" s="6" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="M23" s="16"/>
       <c r="N23" s="16"/>
@@ -13607,7 +13610,7 @@
         <v>3000|54</v>
       </c>
       <c r="L24" s="6" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="M24" s="16"/>
       <c r="N24" s="16"/>
@@ -13670,7 +13673,7 @@
         <v>3500|57</v>
       </c>
       <c r="L25" s="6" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="M25" s="16"/>
       <c r="N25" s="16"/>
@@ -13733,7 +13736,7 @@
         <v>4000|57</v>
       </c>
       <c r="L26" s="6" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="M26" s="16"/>
       <c r="N26" s="16"/>
@@ -13796,7 +13799,7 @@
         <v>4500|56</v>
       </c>
       <c r="L27" s="6" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="M27" s="16"/>
       <c r="N27" s="16"/>
@@ -13859,7 +13862,7 @@
         <v>5000|51</v>
       </c>
       <c r="L28" s="6" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="M28" s="16"/>
       <c r="N28" s="16"/>
@@ -13922,7 +13925,7 @@
         <v>5500|50</v>
       </c>
       <c r="L29" s="6" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="M29" s="16"/>
       <c r="N29" s="16"/>
@@ -13985,7 +13988,7 @@
         <v>6000|46</v>
       </c>
       <c r="L30" s="6" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="M30" s="16"/>
       <c r="N30" s="16"/>
@@ -14048,7 +14051,7 @@
         <v>6500|42</v>
       </c>
       <c r="L31" s="6" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="M31" s="16"/>
       <c r="N31" s="16"/>
@@ -29328,7 +29331,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:X60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>

</xml_diff>